<commit_message>
Update comments, sheet names
</commit_message>
<xml_diff>
--- a/2021-0313846_slurry_separation/EF_calcs/inputs/inputs.xlsx
+++ b/2021-0313846_slurry_separation/EF_calcs/inputs/inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry &amp; application" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Climate" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Application climate" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Separation efficiency" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Storage EFs" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -90,34 +90,6 @@
     <author>SDH</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Sans"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Question: correct to use covered values for these?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Sans"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Correct to use covered values?</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="D4" authorId="0">
       <text>
         <r>
@@ -473,18 +445,18 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="10.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="10.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="9" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="9" style="1" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,7 +908,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>25</v>
       </c>
@@ -1865,13 +1837,13 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1976,17 +1948,17 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="10.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2049,20 +2021,20 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.14453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="10.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Include pH increase 0.2 LF
</commit_message>
<xml_diff>
--- a/2021-0313846_slurry_separation/EF_calcs/inputs/inputs.xlsx
+++ b/2021-0313846_slurry_separation/EF_calcs/inputs/inputs.xlsx
@@ -325,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -351,6 +351,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -446,10 +450,10 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.86"/>
@@ -578,7 +582,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
@@ -595,8 +599,9 @@
         <f aca="false">(1-D5)*E$2</f>
         <v>1.755</v>
       </c>
-      <c r="F5" s="5" t="n">
-        <v>7.2</v>
+      <c r="F5" s="7" t="n">
+        <f aca="false">F$2+0.2</f>
+        <v>7.4</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -608,7 +613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>18</v>
       </c>
@@ -625,8 +630,9 @@
         <f aca="false">(1-D6)*E$3</f>
         <v>2.925</v>
       </c>
-      <c r="F6" s="5" t="n">
-        <v>7</v>
+      <c r="F6" s="7" t="n">
+        <f aca="false">F$3+0.2</f>
+        <v>7.2</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>14</v>
@@ -638,7 +644,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>18</v>
       </c>
@@ -655,8 +661,9 @@
         <f aca="false">(1-D7)*E$4</f>
         <v>2.655</v>
       </c>
-      <c r="F7" s="5" t="n">
-        <v>7.9</v>
+      <c r="F7" s="7" t="n">
+        <f aca="false">F$4+0.2</f>
+        <v>8.1</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
@@ -668,7 +675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>21</v>
       </c>
@@ -685,8 +692,9 @@
         <f aca="false">(1-D8)*E$2</f>
         <v>2.535</v>
       </c>
-      <c r="F8" s="5" t="n">
-        <v>7.2</v>
+      <c r="F8" s="7" t="n">
+        <f aca="false">F$2+0.2</f>
+        <v>7.4</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -698,7 +706,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>21</v>
       </c>
@@ -715,8 +723,9 @@
         <f aca="false">(1-D9)*E$3</f>
         <v>4.225</v>
       </c>
-      <c r="F9" s="5" t="n">
-        <v>7</v>
+      <c r="F9" s="7" t="n">
+        <f aca="false">F$3+0.2</f>
+        <v>7.2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
@@ -728,7 +737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>21</v>
       </c>
@@ -745,8 +754,9 @@
         <f aca="false">(1-D10)*E$4</f>
         <v>3.835</v>
       </c>
-      <c r="F10" s="5" t="n">
-        <v>7.9</v>
+      <c r="F10" s="7" t="n">
+        <f aca="false">F$4+0.2</f>
+        <v>8.1</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -758,7 +768,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>23</v>
       </c>
@@ -775,8 +785,9 @@
         <f aca="false">(1-D11)*E$2</f>
         <v>3.315</v>
       </c>
-      <c r="F11" s="5" t="n">
-        <v>7.2</v>
+      <c r="F11" s="7" t="n">
+        <f aca="false">F$2+0.2</f>
+        <v>7.4</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
@@ -788,7 +799,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>23</v>
       </c>
@@ -805,8 +816,9 @@
         <f aca="false">(1-D12)*E$3</f>
         <v>5.525</v>
       </c>
-      <c r="F12" s="5" t="n">
-        <v>7</v>
+      <c r="F12" s="7" t="n">
+        <f aca="false">F$3+0.2</f>
+        <v>7.2</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
@@ -818,7 +830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>23</v>
       </c>
@@ -835,8 +847,9 @@
         <f aca="false">(1-D13)*E$4</f>
         <v>5.015</v>
       </c>
-      <c r="F13" s="5" t="n">
-        <v>7.9</v>
+      <c r="F13" s="7" t="n">
+        <f aca="false">F$4+0.2</f>
+        <v>8.1</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>14</v>
@@ -848,7 +861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>25</v>
       </c>
@@ -865,8 +878,9 @@
         <f aca="false">(1-D14)*E$2</f>
         <v>3.315</v>
       </c>
-      <c r="F14" s="5" t="n">
-        <v>7.2</v>
+      <c r="F14" s="7" t="n">
+        <f aca="false">F$2+0.2</f>
+        <v>7.4</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>14</v>
@@ -878,7 +892,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>25</v>
       </c>
@@ -895,8 +909,9 @@
         <f aca="false">(1-D15)*E$3</f>
         <v>5.525</v>
       </c>
-      <c r="F15" s="5" t="n">
-        <v>7</v>
+      <c r="F15" s="7" t="n">
+        <f aca="false">F$3+0.2</f>
+        <v>7.2</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>14</v>
@@ -925,8 +940,9 @@
         <f aca="false">(1-D16)*E$4</f>
         <v>5.015</v>
       </c>
-      <c r="F16" s="5" t="n">
-        <v>7.9</v>
+      <c r="F16" s="7" t="n">
+        <f aca="false">F$4+0.2</f>
+        <v>8.1</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
@@ -1837,7 +1853,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8"/>
@@ -1864,13 +1880,13 @@
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="8" t="n">
         <v>4.43101207056639</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="8" t="n">
         <v>4.05891613991413</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="8" t="n">
         <v>0.0599629009095261</v>
       </c>
     </row>
@@ -1878,13 +1894,13 @@
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="8" t="n">
         <v>8.23645983645984</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="8" t="n">
         <v>3.84445591865745</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="8" t="n">
         <v>0.0552119412831931</v>
       </c>
     </row>
@@ -1892,13 +1908,13 @@
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="8" t="n">
         <v>12.4492495309568</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="8" t="n">
         <v>3.48391526295633</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="8" t="n">
         <v>0.0702993488962998</v>
       </c>
     </row>
@@ -1906,13 +1922,13 @@
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="8" t="n">
         <v>16.8762259816193</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <v>3.15624012423227</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="8" t="n">
         <v>0.105925308296069</v>
       </c>
     </row>
@@ -1920,13 +1936,13 @@
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="8" t="n">
         <v>14.4977479635841</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="8" t="n">
         <v>3.32276959833633</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="8" t="n">
         <v>0.128260170445409</v>
       </c>
     </row>
@@ -1952,7 +1968,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.37"/>
@@ -2024,7 +2040,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.57"/>
@@ -2055,17 +2071,17 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="9" t="n">
         <v>0.013</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="9" t="n">
         <v>0.013</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="D2" s="10" t="n">
         <f aca="false">13/0.79/100</f>
         <v>0.164556962025316</v>
       </c>
-      <c r="E2" s="9" t="n">
+      <c r="E2" s="10" t="n">
         <f aca="false">28/0.79/100</f>
         <v>0.354430379746835</v>
       </c>
@@ -2074,17 +2090,17 @@
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="9" t="n">
         <v>0.017</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="9" t="n">
         <v>0.017</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="10" t="n">
         <f aca="false">3/0.58/100</f>
         <v>0.0517241379310345</v>
       </c>
-      <c r="E3" s="9" t="n">
+      <c r="E3" s="10" t="n">
         <f aca="false">13/0.58/100</f>
         <v>0.224137931034483</v>
       </c>
@@ -2093,17 +2109,17 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="9" t="n">
         <v>0.026</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="9" t="n">
         <v>0.026</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="10" t="n">
         <f aca="false">13/0.77/100</f>
         <v>0.168831168831169</v>
       </c>
-      <c r="E4" s="9" t="n">
+      <c r="E4" s="10" t="n">
         <f aca="false">28/0.77/100</f>
         <v>0.363636363636364</v>
       </c>

</xml_diff>